<commit_message>
remade fig3 proteus to contain new chloroplast and cyto protein predcts
</commit_message>
<xml_diff>
--- a/analyses/unipept/lca/T0_322_digested_PeaksDB_lca-mc.xlsx
+++ b/analyses/unipept/lca/T0_322_digested_PeaksDB_lca-mc.xlsx
@@ -5,10 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="T0_322_digested_PeaksDB_lca-mc" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="diatom only" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="diatom cytoplasm protein name" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="diatom membrane protein name" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5192" uniqueCount="3588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6580" uniqueCount="3643">
   <si>
     <t xml:space="preserve">peptide</t>
   </si>
@@ -10784,6 +10787,171 @@
   </si>
   <si>
     <t xml:space="preserve">HSQTPGHP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database protein ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203139294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203628558 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203289348 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|B5A4Q2|B5A4Q2_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203244520 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0171384842 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203505436 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201751422 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203505756 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203628182 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203420370 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203082924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203296644</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203298220 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203275302 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203389878</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protein IDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VNZ5|A0A089VNZ5_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201829098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203287482</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201745788 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201860448</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203603364</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203152572</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203226722</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203172898</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201785164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203265014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKJ4|A0A089VKJ4_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203508352 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0171421366</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203386012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|F2WW93|F2WW93_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203551214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089914|A0A089914_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203255940</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203397068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VQA3|A0A089VQA3_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201742992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VLP5|A0A089VLP5_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203135488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKD8|A0A089VKD8_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203358160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKN5|A0A089VKN5_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203399598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203473996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0171446710</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0201805882</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203608338</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VP49|A0A089VP49_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A089VKJ7|A0A089VKJ7_THAWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203275302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thalassiosira_weissflogii_0203417438</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tr|A0A0898Z4|A0A0898Z4_THAWE</t>
   </si>
 </sst>
 </file>
@@ -10798,6 +10966,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -10857,8 +11026,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -10881,11 +11054,11 @@
   </sheetPr>
   <dimension ref="A1:AW774"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.58"/>
@@ -10895,7 +11068,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.05"/>
@@ -10916,25 +11089,25 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="6.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="39.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="39.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="140.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="88.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="99.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="99.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="82.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="123.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="123.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="166.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="131.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="123.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="155.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="155.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="137.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="121.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="116.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="121.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="0" width="116.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="121.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="53.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="0" width="50.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="0" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="16.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -28070,4 +28243,4496 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AT62"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL2" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH3" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI3" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ3" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK3" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL3" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM3" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN3" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO3" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP3" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH4" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK4" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO4" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP4" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH5" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ5" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK5" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL5" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO5" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP5" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG6" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH6" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI6" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ6" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK6" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL6" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM6" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN6" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO6" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP6" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W7" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA7" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE7" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF7" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG7" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH7" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI7" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="AJ7" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK7" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG8" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH8" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ8" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK8" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL8" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM8" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN8" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO8" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP8" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG9" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="AH9" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="AK9" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL9" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI10" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK10" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL10" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM10" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN10" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO10" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP10" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S11" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W11" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG11" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH11" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="AI11" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="AJ11" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="AM11" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="AN11" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="AO11" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S12" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W12" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG12" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH12" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI12" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ12" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK12" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM12" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO12" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP12" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG13" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="AH13" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="AK13" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL13" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM13" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN13" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="AO13" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP13" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W14" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA14" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="AG14" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="AH14" s="0" t="s">
+        <v>516</v>
+      </c>
+      <c r="AK14" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL14" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM14" s="0" t="s">
+        <v>517</v>
+      </c>
+      <c r="AN14" s="0" t="s">
+        <v>518</v>
+      </c>
+      <c r="AO14" s="0" t="s">
+        <v>519</v>
+      </c>
+      <c r="AP14" s="0" t="s">
+        <v>520</v>
+      </c>
+      <c r="AQ14" s="0" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>522</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S15" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="W15" s="0" t="s">
+        <v>527</v>
+      </c>
+      <c r="AA15" s="0" t="s">
+        <v>523</v>
+      </c>
+      <c r="AK15" s="0" t="s">
+        <v>528</v>
+      </c>
+      <c r="AL15" s="0" t="s">
+        <v>529</v>
+      </c>
+      <c r="AM15" s="0" t="s">
+        <v>530</v>
+      </c>
+      <c r="AN15" s="0" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S16" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W16" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH17" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI17" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ17" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK17" s="0" t="s">
+        <v>600</v>
+      </c>
+      <c r="AL17" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM17" s="0" t="s">
+        <v>601</v>
+      </c>
+      <c r="AN17" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO17" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP17" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S18" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W18" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA18" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG18" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH18" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI18" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ18" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK18" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL18" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM18" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN18" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO18" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP18" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S19" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W19" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA19" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="AI19" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="AJ19" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="AM19" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="AN19" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="AO19" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="AP19" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="AQ19" s="0" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S20" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W20" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA20" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG20" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH20" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI20" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ20" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK20" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL20" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM20" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN20" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO20" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP20" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE21" s="0" t="s">
+        <v>412</v>
+      </c>
+      <c r="AF21" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="AG21" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="AH21" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="AI21" s="0" t="s">
+        <v>724</v>
+      </c>
+      <c r="AJ21" s="0" t="s">
+        <v>725</v>
+      </c>
+      <c r="AM21" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="AN21" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="AO21" s="0" t="s">
+        <v>728</v>
+      </c>
+      <c r="AP21" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S22" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W22" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG22" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="AH22" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="AM22" s="0" t="s">
+        <v>807</v>
+      </c>
+      <c r="AN22" s="0" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG23" s="0" t="s">
+        <v>833</v>
+      </c>
+      <c r="AH23" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="AI23" s="0" t="s">
+        <v>835</v>
+      </c>
+      <c r="AJ23" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="AK23" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="AL23" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="AM23" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="AN23" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="AO23" s="0" t="s">
+        <v>841</v>
+      </c>
+      <c r="AP23" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="AQ23" s="0" t="s">
+        <v>843</v>
+      </c>
+      <c r="AR23" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="AS23" s="0" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="W24" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="AA24" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="AI24" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="AJ24" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="AK24" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN24" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="AO24" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="AP24" s="0" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W25" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA25" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG25" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="AH25" s="0" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG26" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="AH26" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE27" s="0" t="s">
+        <v>995</v>
+      </c>
+      <c r="AF27" s="0" t="s">
+        <v>996</v>
+      </c>
+      <c r="AI27" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="AJ27" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK27" s="0" t="s">
+        <v>997</v>
+      </c>
+      <c r="AL27" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="AM27" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="AN27" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="AO27" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="AP27" s="0" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W28" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA28" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE28" s="0" t="s">
+        <v>1004</v>
+      </c>
+      <c r="AF28" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="AG28" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="AH28" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="AI28" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="AJ28" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="AK28" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="AL28" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="AM28" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="AN28" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="AO28" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S29" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W29" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA29" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE29" s="0" t="s">
+        <v>1014</v>
+      </c>
+      <c r="AF29" s="0" t="s">
+        <v>1015</v>
+      </c>
+      <c r="AI29" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="AJ29" s="0" t="s">
+        <v>1017</v>
+      </c>
+      <c r="AK29" s="0" t="s">
+        <v>1018</v>
+      </c>
+      <c r="AL29" s="0" t="s">
+        <v>1019</v>
+      </c>
+      <c r="AM29" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="AN29" s="0" t="s">
+        <v>1021</v>
+      </c>
+      <c r="AO29" s="0" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S30" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W30" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA30" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG30" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="AH30" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="AI30" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AJ30" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AK30" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AL30" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AM30" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="AN30" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="AO30" s="0" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG31" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="AH31" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="AI31" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="AJ31" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="AK31" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="AL31" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="AM31" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="AN31" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="AO31" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="AP31" s="0" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="S32" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="W32" s="0" t="s">
+        <v>1151</v>
+      </c>
+      <c r="AA32" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="AE32" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF32" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="AG32" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH32" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI32" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="AJ32" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="AK32" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN32" s="0" t="s">
+        <v>379</v>
+      </c>
+      <c r="AO32" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="AP32" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N33" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S33" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W33" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA33" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG33" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="AH33" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="AI33" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AJ33" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AK33" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AL33" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AM33" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="AN33" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="AO33" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="AP33" s="0" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S34" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W34" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N35" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S35" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W35" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="S36" s="0" t="s">
+        <v>1150</v>
+      </c>
+      <c r="W36" s="0" t="s">
+        <v>1226</v>
+      </c>
+      <c r="AA36" s="0" t="s">
+        <v>1225</v>
+      </c>
+      <c r="AG36" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="AH36" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="AI36" s="0" t="s">
+        <v>1229</v>
+      </c>
+      <c r="AJ36" s="0" t="s">
+        <v>1230</v>
+      </c>
+      <c r="AM36" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="AN36" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="AO36" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP36" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="AQ36" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="AR36" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE37" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="AF37" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG37" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH37" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI37" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="AJ37" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK37" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL37" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="AM37" s="0" t="s">
+        <v>590</v>
+      </c>
+      <c r="AN37" s="0" t="s">
+        <v>591</v>
+      </c>
+      <c r="AO37" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N38" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S38" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W38" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA38" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG38" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH38" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI38" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ38" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK38" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL38" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM38" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN38" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO38" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP38" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N39" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W39" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG39" s="0" t="s">
+        <v>1390</v>
+      </c>
+      <c r="AH39" s="0" t="s">
+        <v>1391</v>
+      </c>
+      <c r="AI39" s="0" t="s">
+        <v>1392</v>
+      </c>
+      <c r="AJ39" s="0" t="s">
+        <v>1393</v>
+      </c>
+      <c r="AK39" s="0" t="s">
+        <v>1394</v>
+      </c>
+      <c r="AL39" s="0" t="s">
+        <v>1395</v>
+      </c>
+      <c r="AM39" s="0" t="s">
+        <v>1396</v>
+      </c>
+      <c r="AN39" s="0" t="s">
+        <v>1397</v>
+      </c>
+      <c r="AO39" s="0" t="s">
+        <v>1398</v>
+      </c>
+      <c r="AP39" s="0" t="s">
+        <v>1399</v>
+      </c>
+      <c r="AQ39" s="0" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N40" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S40" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W40" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA40" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="AG40" s="0" t="s">
+        <v>1434</v>
+      </c>
+      <c r="AH40" s="0" t="s">
+        <v>1435</v>
+      </c>
+      <c r="AI40" s="0" t="s">
+        <v>1436</v>
+      </c>
+      <c r="AJ40" s="0" t="s">
+        <v>1437</v>
+      </c>
+      <c r="AK40" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL40" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="AM40" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="AN40" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N41" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S41" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="W41" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="AA41" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="AG41" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH41" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI41" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ41" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK41" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL41" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM41" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N42" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S42" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W42" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA42" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AI42" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="AJ42" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="AK42" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="AL42" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="AM42" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="AN42" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="AO42" s="0" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG43" s="0" t="s">
+        <v>1607</v>
+      </c>
+      <c r="AH43" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="AI43" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="AJ43" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="AK43" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AL43" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AM43" s="0" t="s">
+        <v>1609</v>
+      </c>
+      <c r="AN43" s="0" t="s">
+        <v>1610</v>
+      </c>
+      <c r="AO43" s="0" t="s">
+        <v>1611</v>
+      </c>
+      <c r="AP43" s="0" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K44" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N44" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG44" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="AH44" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="AM44" s="0" t="s">
+        <v>726</v>
+      </c>
+      <c r="AN44" s="0" t="s">
+        <v>727</v>
+      </c>
+      <c r="AO44" s="0" t="s">
+        <v>728</v>
+      </c>
+      <c r="AP44" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K45" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N45" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG45" s="0" t="s">
+        <v>1762</v>
+      </c>
+      <c r="AH45" s="0" t="s">
+        <v>1763</v>
+      </c>
+      <c r="AI45" s="0" t="s">
+        <v>1764</v>
+      </c>
+      <c r="AJ45" s="0" t="s">
+        <v>1765</v>
+      </c>
+      <c r="AK45" s="0" t="s">
+        <v>1766</v>
+      </c>
+      <c r="AL45" s="0" t="s">
+        <v>1767</v>
+      </c>
+      <c r="AM45" s="0" t="s">
+        <v>1768</v>
+      </c>
+      <c r="AN45" s="0" t="s">
+        <v>1769</v>
+      </c>
+      <c r="AO45" s="0" t="s">
+        <v>1770</v>
+      </c>
+      <c r="AP45" s="0" t="s">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG46" s="0" t="s">
+        <v>1950</v>
+      </c>
+      <c r="AH46" s="0" t="s">
+        <v>1951</v>
+      </c>
+      <c r="AI46" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AJ46" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AK46" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AL46" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AM46" s="0" t="s">
+        <v>1952</v>
+      </c>
+      <c r="AN46" s="0" t="s">
+        <v>1953</v>
+      </c>
+      <c r="AO46" s="0" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG47" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="AH47" s="0" t="s">
+        <v>723</v>
+      </c>
+      <c r="AI47" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="AJ47" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="AK47" s="0" t="s">
+        <v>1973</v>
+      </c>
+      <c r="AL47" s="0" t="s">
+        <v>1974</v>
+      </c>
+      <c r="AM47" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="AN47" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="AO47" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="AP47" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="AQ47" s="0" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K48" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N48" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S48" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W48" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA48" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG48" s="0" t="s">
+        <v>1976</v>
+      </c>
+      <c r="AH48" s="0" t="s">
+        <v>1977</v>
+      </c>
+      <c r="AK48" s="0" t="s">
+        <v>1978</v>
+      </c>
+      <c r="AL48" s="0" t="s">
+        <v>1979</v>
+      </c>
+      <c r="AM48" s="0" t="s">
+        <v>1980</v>
+      </c>
+      <c r="AN48" s="0" t="s">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N49" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S49" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="W49" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="AA49" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="AG49" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH49" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI49" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ49" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK49" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL49" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM49" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN49" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO49" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP49" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>2173</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="AI50" s="0" t="s">
+        <v>2174</v>
+      </c>
+      <c r="AJ50" s="0" t="s">
+        <v>2175</v>
+      </c>
+      <c r="AK50" s="0" t="s">
+        <v>2176</v>
+      </c>
+      <c r="AL50" s="0" t="s">
+        <v>2177</v>
+      </c>
+      <c r="AM50" s="0" t="s">
+        <v>2178</v>
+      </c>
+      <c r="AN50" s="0" t="s">
+        <v>2179</v>
+      </c>
+      <c r="AO50" s="0" t="s">
+        <v>2180</v>
+      </c>
+      <c r="AP50" s="0" t="s">
+        <v>2181</v>
+      </c>
+      <c r="AQ50" s="0" t="s">
+        <v>2182</v>
+      </c>
+      <c r="AR50" s="0" t="s">
+        <v>2183</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K51" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N51" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S51" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W51" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE51" s="0" t="s">
+        <v>2446</v>
+      </c>
+      <c r="AF51" s="0" t="s">
+        <v>2447</v>
+      </c>
+      <c r="AG51" s="0" t="s">
+        <v>2448</v>
+      </c>
+      <c r="AH51" s="0" t="s">
+        <v>2449</v>
+      </c>
+      <c r="AI51" s="0" t="s">
+        <v>2450</v>
+      </c>
+      <c r="AJ51" s="0" t="s">
+        <v>2451</v>
+      </c>
+      <c r="AK51" s="0" t="s">
+        <v>2452</v>
+      </c>
+      <c r="AN51" s="0" t="s">
+        <v>2453</v>
+      </c>
+      <c r="AO51" s="0" t="s">
+        <v>2454</v>
+      </c>
+      <c r="AP51" s="0" t="s">
+        <v>2455</v>
+      </c>
+      <c r="AQ51" s="0" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG52" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH52" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI52" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ52" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK52" s="0" t="s">
+        <v>2495</v>
+      </c>
+      <c r="AL52" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="AM52" s="0" t="s">
+        <v>2496</v>
+      </c>
+      <c r="AN52" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO52" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP52" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N53" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S53" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="W53" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="AA53" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="AG53" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH53" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI53" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ53" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK53" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL53" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM53" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN53" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO53" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP53" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N54" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S54" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W54" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG55" s="0" t="s">
+        <v>3002</v>
+      </c>
+      <c r="AH55" s="0" t="s">
+        <v>3003</v>
+      </c>
+      <c r="AI55" s="0" t="s">
+        <v>3004</v>
+      </c>
+      <c r="AJ55" s="0" t="s">
+        <v>3005</v>
+      </c>
+      <c r="AK55" s="0" t="s">
+        <v>837</v>
+      </c>
+      <c r="AL55" s="0" t="s">
+        <v>3006</v>
+      </c>
+      <c r="AM55" s="0" t="s">
+        <v>839</v>
+      </c>
+      <c r="AN55" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="AO55" s="0" t="s">
+        <v>3007</v>
+      </c>
+      <c r="AP55" s="0" t="s">
+        <v>1317</v>
+      </c>
+      <c r="AQ55" s="0" t="s">
+        <v>3008</v>
+      </c>
+      <c r="AR55" s="0" t="s">
+        <v>3009</v>
+      </c>
+      <c r="AS55" s="0" t="s">
+        <v>3010</v>
+      </c>
+      <c r="AT55" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N56" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S56" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W56" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA56" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG56" s="0" t="s">
+        <v>3117</v>
+      </c>
+      <c r="AH56" s="0" t="s">
+        <v>3118</v>
+      </c>
+      <c r="AI56" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="AJ56" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="AK56" s="0" t="s">
+        <v>3119</v>
+      </c>
+      <c r="AL56" s="0" t="s">
+        <v>3120</v>
+      </c>
+      <c r="AM56" s="0" t="s">
+        <v>1384</v>
+      </c>
+      <c r="AN56" s="0" t="s">
+        <v>3121</v>
+      </c>
+      <c r="AO56" s="0" t="s">
+        <v>1952</v>
+      </c>
+      <c r="AP56" s="0" t="s">
+        <v>1953</v>
+      </c>
+      <c r="AQ56" s="0" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG57" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH57" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="AK57" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL57" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>3197</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N58" s="0" t="s">
+        <v>525</v>
+      </c>
+      <c r="S58" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="AG58" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH58" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI58" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ58" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK58" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL58" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM58" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN58" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO58" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="AP58" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>524</v>
+      </c>
+      <c r="N59" s="0" t="s">
+        <v>1149</v>
+      </c>
+      <c r="S59" s="0" t="s">
+        <v>3382</v>
+      </c>
+      <c r="W59" s="0" t="s">
+        <v>3383</v>
+      </c>
+      <c r="AA59" s="0" t="s">
+        <v>3381</v>
+      </c>
+      <c r="AG59" s="0" t="s">
+        <v>3384</v>
+      </c>
+      <c r="AH59" s="0" t="s">
+        <v>3385</v>
+      </c>
+      <c r="AI59" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="AJ59" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="AK59" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="AL59" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="AM59" s="0" t="s">
+        <v>3386</v>
+      </c>
+      <c r="AN59" s="0" t="s">
+        <v>3387</v>
+      </c>
+      <c r="AO59" s="0" t="s">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>3422</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N60" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S60" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W60" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA60" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="AG60" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH60" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI60" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ60" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK60" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL60" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM60" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>3522</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE61" s="0" t="s">
+        <v>979</v>
+      </c>
+      <c r="AF61" s="0" t="s">
+        <v>980</v>
+      </c>
+      <c r="AG61" s="0" t="s">
+        <v>3523</v>
+      </c>
+      <c r="AH61" s="0" t="s">
+        <v>3524</v>
+      </c>
+      <c r="AI61" s="0" t="s">
+        <v>3525</v>
+      </c>
+      <c r="AJ61" s="0" t="s">
+        <v>3526</v>
+      </c>
+      <c r="AK61" s="0" t="s">
+        <v>3527</v>
+      </c>
+      <c r="AL61" s="0" t="s">
+        <v>3528</v>
+      </c>
+      <c r="AM61" s="0" t="s">
+        <v>3529</v>
+      </c>
+      <c r="AN61" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="AO61" s="0" t="s">
+        <v>3530</v>
+      </c>
+      <c r="AP61" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>3555</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="N62" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="S62" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="W62" s="0" t="s">
+        <v>514</v>
+      </c>
+      <c r="AA62" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="AG62" s="0" t="s">
+        <v>3556</v>
+      </c>
+      <c r="AH62" s="0" t="s">
+        <v>3557</v>
+      </c>
+      <c r="AI62" s="0" t="s">
+        <v>1436</v>
+      </c>
+      <c r="AJ62" s="0" t="s">
+        <v>1437</v>
+      </c>
+      <c r="AK62" s="0" t="s">
+        <v>3558</v>
+      </c>
+      <c r="AL62" s="0" t="s">
+        <v>3559</v>
+      </c>
+      <c r="AM62" s="0" t="s">
+        <v>3560</v>
+      </c>
+      <c r="AN62" s="0" t="s">
+        <v>3561</v>
+      </c>
+      <c r="AO62" s="0" t="s">
+        <v>3562</v>
+      </c>
+      <c r="AP62" s="0" t="s">
+        <v>3563</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="40.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="70.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="41.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="33.8"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3588</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3589</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>679</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3590</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>682</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>684</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>685</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3591</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>873</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>994</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>3592</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>680</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>681</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>997</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>998</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>683</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>1000</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3593</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>981</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>1008</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>3594</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>1016</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>1017</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>1019</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>1021</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3595</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>1129</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>1130</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>1133</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3596</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>1141</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>1142</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>1143</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>1144</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>1145</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>3595</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>1196</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>1197</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>1198</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>1134</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>1199</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>3597</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>3598</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>3599</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>1531</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>1532</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>1533</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>1534</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>1535</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>1536</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>3600</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>1607</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>1609</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>1610</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>1611</v>
+      </c>
+      <c r="M14" s="0" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>2883</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>3602</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>3117</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>3118</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>3119</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>3120</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>1384</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>3121</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>1952</v>
+      </c>
+      <c r="M16" s="0" t="s">
+        <v>1953</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>3603</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>3384</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>3385</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>3386</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>3387</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>3522</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>3604</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>3523</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>3524</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>3525</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>3526</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>3527</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>3528</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>3529</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>988</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>3530</v>
+      </c>
+      <c r="M18" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H42"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3605</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3606</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3607</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3608</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>3609</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3610</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>3611</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3612</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3613</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>3614</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>3615</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>469</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>3616</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>486</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>3613</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>512</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>3617</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>515</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>599</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>3618</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>668</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>3619</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>687</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>3620</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>721</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>3621</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>3622</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>3623</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>833</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>3624</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>3625</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>383</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>3611</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>3626</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>1227</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3606</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>3627</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>3628</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>1434</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>1487</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>3629</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>1624</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>3630</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>3631</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>1762</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>3632</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>722</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>3633</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>1976</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>2156</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>3634</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>2445</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>3635</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>2448</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>2494</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>3636</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>2730</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>3637</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>3001</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>3638</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>3002</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>3003</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>3009</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>3010</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>3639</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>3197</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>526</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>3631</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>3640</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>3384</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>3422</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>3641</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>3555</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>513</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>3642</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>3556</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>3557</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>